<commit_message>
Added more movies and reviews.
</commit_message>
<xml_diff>
--- a/movies_list.xlsx
+++ b/movies_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="67">
   <si>
     <t xml:space="preserve">genre</t>
   </si>
@@ -34,21 +34,51 @@
     <t xml:space="preserve">Action</t>
   </si>
   <si>
+    <t xml:space="preserve">Goldfinger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Wild Bunch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter the Dragon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Star Wars: Episode IV - A New Hope</t>
   </si>
   <si>
+    <t xml:space="preserve">Commando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lethal Weapon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RoboCop</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indiana Jones and the Last Crusade</t>
   </si>
   <si>
+    <t xml:space="preserve">Speed</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Matrix</t>
   </si>
   <si>
     <t xml:space="preserve">Fight Club</t>
   </si>
   <si>
+    <t xml:space="preserve">Crouching Tiger, Hidden Dragon</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Departed</t>
   </si>
   <si>
+    <t xml:space="preserve">Inception</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Wick</t>
+  </si>
+  <si>
     <t xml:space="preserve">Horror</t>
   </si>
   <si>
@@ -58,18 +88,51 @@
     <t xml:space="preserve">The Exorcist</t>
   </si>
   <si>
+    <t xml:space="preserve">The Omen</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Shining</t>
   </si>
   <si>
+    <t xml:space="preserve">Poltergeist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Nightmare on Elm Street</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Silence of the Lambs</t>
   </si>
   <si>
+    <t xml:space="preserve">Scream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Blair Witch Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Grudge</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Conjuring</t>
   </si>
   <si>
+    <t xml:space="preserve">It Follows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It</t>
+  </si>
+  <si>
     <t xml:space="preserve">Romance</t>
   </si>
   <si>
+    <t xml:space="preserve">Roman Holiday</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Graduate</t>
   </si>
   <si>
@@ -79,9 +142,33 @@
     <t xml:space="preserve">Pretty Woman</t>
   </si>
   <si>
+    <t xml:space="preserve">Jerry Maguire</t>
+  </si>
+  <si>
     <t xml:space="preserve">Titanic</t>
   </si>
   <si>
+    <t xml:space="preserve">You've Got Mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notting Hill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serendipity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Walk to Remember</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Notebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 First Dates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 Days of Summer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Silver Linings Playbook</t>
   </si>
   <si>
@@ -94,21 +181,55 @@
     <t xml:space="preserve">Caddyshack</t>
   </si>
   <si>
+    <t xml:space="preserve">The Mighty Ducks</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cool Runnings</t>
   </si>
   <si>
+    <t xml:space="preserve">Tin Cup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any Given Sunday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remember the Titans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bend It like Beckham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seabiscuit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miracle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Million Dollar Baby</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Greatest Game Ever Played</t>
   </si>
   <si>
-    <t xml:space="preserve">The Blind Side </t>
+    <t xml:space="preserve">Coach Carter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Blind Side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moneyball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rush</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -186,12 +307,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -212,7 +341,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -221,8 +350,8 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6632653061225"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -245,7 +374,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1977</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -256,7 +385,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>1989</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -267,7 +396,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>1999</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,7 +407,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>1999</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -289,172 +418,613 @@
         <v>8</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2006</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" s="0" t="n">
-        <v>1960</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>1973</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>1980</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>1991</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>2013</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>1967</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="C13" s="0" t="n">
-        <v>1989</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>1990</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>1997</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>2012</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>1976</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="C18" s="0" t="n">
-        <v>1980</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>1993</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>2005</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C23" s="0" t="n">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>1998</v>
+      </c>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="0" t="n">
         <v>2009</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>2013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>